<commit_message>
Before Break: SARSA and Q-Learning experiment done, finding out why results are same for them?
</commit_message>
<xml_diff>
--- a/Faa_neew/p11-faa-0ms.xlsx
+++ b/Faa_neew/p11-faa-0ms.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens interaction logs\annotated\Faa-0ms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\Faa_neew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB748ECF-C01C-4502-A191-870A24DB8D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6582ED2-2F1D-4E16-A6D4-2CBD77ADBA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet(2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="90">
   <si>
     <t>proposition</t>
   </si>
@@ -292,6 +293,15 @@
   </si>
   <si>
     <t>Reward</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>steer</t>
+  </si>
+  <si>
+    <t>explanation</t>
   </si>
 </sst>
 </file>
@@ -658,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -2414,4 +2424,1967 @@
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F29AB1-AF8E-4CC9-A92E-8FDDCED8D38F}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:K66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="116.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="4" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="9" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="38.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1.8518518518518518E-4</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2.8935185185185184E-4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>3.3564814814814812E-4</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5.2083333333333333E-4</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>5.5555555555555556E-4</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>7.291666666666667E-4</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>7.7546296296296293E-4</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>8.6805555555555551E-4</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.0069444444444444E-3</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.0532407407407407E-3</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1.0995370370370371E-3</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>1.261574074074074E-3</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>2</v>
+      </c>
+      <c r="I14" s="2">
+        <v>1.3425925925925925E-3</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1.4351851851851852E-3</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1.5393518518518519E-3</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>1.736111111111111E-3</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.9212962962962964E-3</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>2.1759259259259258E-3</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" s="2">
+        <v>2.2916666666666667E-3</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>2</v>
+      </c>
+      <c r="I22" s="2">
+        <v>2.3379629629629631E-3</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2.5115740740740741E-3</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2.5231481481481481E-3</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2.5810185185185185E-3</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>2.673611111111111E-3</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="2">
+        <v>2.8819444444444444E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>2.9282407407407408E-3</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3.7962962962962963E-3</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2</v>
+      </c>
+      <c r="I30" s="2">
+        <v>3.8425925925925928E-3</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" s="2">
+        <v>3.8657407407407408E-3</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>2</v>
+      </c>
+      <c r="I32" s="2">
+        <v>4.0393518518518521E-3</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>2</v>
+      </c>
+      <c r="I33" s="2">
+        <v>4.31712962962963E-3</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>4.4791666666666669E-3</v>
+      </c>
+      <c r="J34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>2</v>
+      </c>
+      <c r="I35" s="2">
+        <v>4.5833333333333334E-3</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>4.6643518518518518E-3</v>
+      </c>
+      <c r="J36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>4.6990740740740743E-3</v>
+      </c>
+      <c r="J37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2</v>
+      </c>
+      <c r="I38" s="2">
+        <v>4.7800925925925927E-3</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2</v>
+      </c>
+      <c r="I39" s="2">
+        <v>4.9074074074074072E-3</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2">
+        <v>4.9768518518518521E-3</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>2</v>
+      </c>
+      <c r="I41" s="2">
+        <v>5.0115740740740737E-3</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1">
+        <v>2</v>
+      </c>
+      <c r="I42" s="2">
+        <v>5.0578703703703706E-3</v>
+      </c>
+      <c r="J42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2</v>
+      </c>
+      <c r="I43" s="2">
+        <v>5.162037037037037E-3</v>
+      </c>
+      <c r="J43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2</v>
+      </c>
+      <c r="I44" s="2">
+        <v>5.4629629629629629E-3</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1">
+        <v>2</v>
+      </c>
+      <c r="I45" s="2">
+        <v>5.5324074074074078E-3</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+      <c r="G46" s="1">
+        <v>2</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1">
+        <v>2</v>
+      </c>
+      <c r="I47" s="2">
+        <v>5.6481481481481478E-3</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="I48" s="2">
+        <v>5.8449074074074072E-3</v>
+      </c>
+      <c r="J48">
+        <v>4</v>
+      </c>
+      <c r="K48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="1">
+        <v>2</v>
+      </c>
+      <c r="G49" s="1">
+        <v>2</v>
+      </c>
+      <c r="I49" s="2">
+        <v>6.0185185185185185E-3</v>
+      </c>
+      <c r="J49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+      <c r="G50" s="1">
+        <v>2</v>
+      </c>
+      <c r="I50" s="2">
+        <v>6.1342592592592594E-3</v>
+      </c>
+      <c r="J50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+      <c r="I51" s="2">
+        <v>6.4236111111111108E-3</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2">
+        <v>6.5624999999999998E-3</v>
+      </c>
+      <c r="J52">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="I53" s="2">
+        <v>7.013888888888889E-3</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>2</v>
+      </c>
+      <c r="I54" s="2">
+        <v>7.1759259259259259E-3</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1">
+        <v>2</v>
+      </c>
+      <c r="I55" s="2">
+        <v>7.2569444444444443E-3</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1">
+        <v>2</v>
+      </c>
+      <c r="I56" s="2">
+        <v>7.2800925925925923E-3</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="1">
+        <v>0</v>
+      </c>
+      <c r="G57" s="1">
+        <v>2</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I57" s="2">
+        <v>7.3032407407407404E-3</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C58" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>2</v>
+      </c>
+      <c r="I58" s="2">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="J58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>2</v>
+      </c>
+      <c r="I59" s="2">
+        <v>7.6157407407407406E-3</v>
+      </c>
+      <c r="J59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="1">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2">
+        <v>7.6504629629629631E-3</v>
+      </c>
+      <c r="J60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>2</v>
+      </c>
+      <c r="I61" s="2">
+        <v>7.7546296296296295E-3</v>
+      </c>
+      <c r="J61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C62" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>2</v>
+      </c>
+      <c r="I62" s="2">
+        <v>7.789351851851852E-3</v>
+      </c>
+      <c r="J62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B63" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="2">
+        <v>7.8472222222222224E-3</v>
+      </c>
+      <c r="J63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" s="1">
+        <v>0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="2">
+        <v>7.9282407407407409E-3</v>
+      </c>
+      <c r="J64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1">
+        <v>2</v>
+      </c>
+      <c r="I65" s="2">
+        <v>7.9629629629629634E-3</v>
+      </c>
+      <c r="J65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B66" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1">
+        <v>2</v>
+      </c>
+      <c r="I66" s="2">
+        <v>8.0902777777777778E-3</v>
+      </c>
+      <c r="J66">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+</worksheet>
 </file>
</xml_diff>